<commit_message>
Added UNO EmptyApp Startup time
</commit_message>
<xml_diff>
--- a/data/chatapp-startup.xlsx
+++ b/data/chatapp-startup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\cross-platform-performance\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A22505C-2129-4E6E-95D7-5966248C05CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46583B85-91D8-48E5-A905-F2531030EF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,6 +391,9 @@
                 <c:pt idx="2">
                   <c:v>257.39999999999998</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>1910.2</c:v>
+                </c:pt>
                 <c:pt idx="4">
                   <c:v>377</c:v>
                 </c:pt>
@@ -1423,7 +1426,7 @@
   <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1479,9 @@
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5">
+        <v>1910.2</v>
+      </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">

</xml_diff>